<commit_message>
W update logs import
</commit_message>
<xml_diff>
--- a/public/images/uploads/import_file_full.xlsx
+++ b/public/images/uploads/import_file_full.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\momo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\stock\public\images\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -209,15 +209,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>DW</t>
-  </si>
-  <si>
-    <t>side</t>
-  </si>
-  <si>
-    <t>symbol</t>
-  </si>
-  <si>
     <t>volume</t>
   </si>
   <si>
@@ -230,16 +221,25 @@
     <t>amount</t>
   </si>
   <si>
-    <t>atpay</t>
-  </si>
-  <si>
-    <t>netamount</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>broker</t>
+    <t>side_id</t>
+  </si>
+  <si>
+    <t>symbol_id</t>
+  </si>
+  <si>
+    <t>at_pay</t>
+  </si>
+  <si>
+    <t>net_amount</t>
+  </si>
+  <si>
+    <t>broker_id</t>
+  </si>
+  <si>
+    <t>is_dw</t>
   </si>
 </sst>
 </file>
@@ -627,37 +627,39 @@
   <dimension ref="A1:L746"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>68</v>
@@ -666,13 +668,13 @@
         <v>69</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>